<commit_message>
Page id model improved to include appendix keyword, tokeniser not including all keywords fixed
</commit_message>
<xml_diff>
--- a/textracting/datasets/identified_trans_marginals_dataset.xlsx
+++ b/textracting/datasets/identified_trans_marginals_dataset.xlsx
@@ -84,9 +84,6 @@
     <t xml:space="preserve">word word word word word tab smallNum tab month bigNum </t>
   </si>
   <si>
-    <t xml:space="preserve">word word bigNum tab word word word tab word </t>
-  </si>
-  <si>
     <t xml:space="preserve">word word word word tab smallNum </t>
   </si>
   <si>
@@ -1065,18 +1062,9 @@
     <t xml:space="preserve">word word word smallNum word word tab page word smallNum </t>
   </si>
   <si>
-    <t xml:space="preserve">mix word smallNum word word word smallNum word smallNum </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mix word smallNum word word word smallNum tab word smallNum </t>
-  </si>
-  <si>
     <t xml:space="preserve">month bigNum tab smallNum </t>
   </si>
   <si>
-    <t xml:space="preserve">mix word smallNum word word word smallNum tab word tab word smallNum </t>
-  </si>
-  <si>
     <t xml:space="preserve">word word word word tab word </t>
   </si>
   <si>
@@ -1111,6 +1099,18 @@
   </si>
   <si>
     <t xml:space="preserve">word bigNum word tab month bigNum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mix word smallNum word word word smallNum appendix smallNum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mix word smallNum word word word smallNum tab appendix smallNum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mix word smallNum word word word smallNum tab word tab appendix smallNum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">word word bigNum tab word word word tab appendix </t>
   </si>
 </sst>
 </file>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C485"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,13 +1931,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B1" t="s">
         <v>344</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>345</v>
-      </c>
-      <c r="C1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2096,7 +2096,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -2272,7 +2272,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -2393,7 +2393,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
@@ -2503,7 +2503,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B57" t="s">
         <v>11</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -2613,7 +2613,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
@@ -2668,7 +2668,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B69" t="s">
         <v>11</v>
@@ -2690,10 +2690,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B70" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -2701,10 +2701,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2712,10 +2712,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2723,10 +2723,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2734,10 +2734,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B76" t="s">
         <v>2</v>
@@ -2767,10 +2767,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -2789,7 +2789,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -2822,10 +2822,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B82" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2833,10 +2833,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B83" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B84" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -2855,10 +2855,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B85" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -2866,10 +2866,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B86" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -2877,10 +2877,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B87" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -2888,10 +2888,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -2899,10 +2899,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -2910,10 +2910,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B90" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -2921,10 +2921,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B91" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -2932,10 +2932,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B92" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -2943,10 +2943,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B93" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -2954,10 +2954,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B94" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -2965,10 +2965,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B95" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -2976,10 +2976,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B96" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2987,10 +2987,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B97" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -2998,10 +2998,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B98" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -3009,10 +3009,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -3020,10 +3020,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B100" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -3031,10 +3031,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B101" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -3042,10 +3042,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B102" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -3053,10 +3053,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B103" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -3064,10 +3064,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B104" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -3075,10 +3075,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B105" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -3097,10 +3097,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B107" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -3108,10 +3108,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B108" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -3119,10 +3119,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B109" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -3130,10 +3130,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B110" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -3141,10 +3141,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B111" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -3152,10 +3152,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B112" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -3163,10 +3163,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B113" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -3174,10 +3174,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B114" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -3185,10 +3185,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B115" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -3196,10 +3196,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B116" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B117" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B118" t="s">
         <v>3</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B119" t="s">
         <v>3</v>
@@ -3240,10 +3240,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B120" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -3251,10 +3251,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B121" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -3262,10 +3262,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -3273,10 +3273,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B123" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3284,10 +3284,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B124" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -3295,10 +3295,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B125" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -3306,10 +3306,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B126" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -3317,10 +3317,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B127" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -3328,10 +3328,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B128" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -3339,10 +3339,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B129" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -3350,10 +3350,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B130" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -3361,10 +3361,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B131" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B132" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -3383,10 +3383,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B133" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -3394,10 +3394,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B134" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -3405,10 +3405,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B135" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -3416,10 +3416,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B136" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -3427,10 +3427,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B137" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -3438,10 +3438,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B138" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -3449,10 +3449,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B139" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -3460,10 +3460,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B140" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -3482,10 +3482,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B142" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3493,10 +3493,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B143" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -3504,10 +3504,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B144" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -3515,10 +3515,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B145" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B146" t="s">
         <v>2</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B147" t="s">
         <v>2</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B148" t="s">
         <v>2</v>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B149" t="s">
         <v>2</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B150" t="s">
         <v>2</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B151" t="s">
         <v>2</v>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B152" t="s">
         <v>2</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B153" t="s">
         <v>2</v>
@@ -3614,7 +3614,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B154" t="s">
         <v>1</v>
@@ -3625,7 +3625,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B155" t="s">
         <v>2</v>
@@ -3636,7 +3636,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B156" t="s">
         <v>2</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B157" t="s">
         <v>2</v>
@@ -3658,7 +3658,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B158" t="s">
         <v>2</v>
@@ -3669,7 +3669,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B159" t="s">
         <v>4</v>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B160" t="s">
         <v>4</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B161" t="s">
         <v>4</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B162" t="s">
         <v>4</v>
@@ -3713,7 +3713,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B163" t="s">
         <v>4</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B164" t="s">
         <v>4</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B165" t="s">
         <v>2</v>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B166" t="s">
         <v>4</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B167" t="s">
         <v>4</v>
@@ -3768,7 +3768,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B168" t="s">
         <v>4</v>
@@ -3779,7 +3779,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B169" t="s">
         <v>4</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B170" t="s">
         <v>4</v>
@@ -3801,7 +3801,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B171" t="s">
         <v>4</v>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B172" t="s">
         <v>4</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B173" t="s">
         <v>4</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B174" t="s">
         <v>4</v>
@@ -3845,7 +3845,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B175" t="s">
         <v>4</v>
@@ -3856,7 +3856,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B176" t="s">
         <v>4</v>
@@ -3867,7 +3867,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B177" t="s">
         <v>4</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B178" t="s">
         <v>4</v>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B179" t="s">
         <v>4</v>
@@ -3900,7 +3900,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B180" t="s">
         <v>4</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B181" t="s">
         <v>4</v>
@@ -3922,7 +3922,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B182" t="s">
         <v>4</v>
@@ -3933,7 +3933,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B183" t="s">
         <v>4</v>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B184" t="s">
         <v>2</v>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B185" t="s">
         <v>4</v>
@@ -3966,7 +3966,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B186" t="s">
         <v>4</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B187" t="s">
         <v>4</v>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B188" t="s">
         <v>4</v>
@@ -3999,7 +3999,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B189" t="s">
         <v>2</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B190" t="s">
         <v>4</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B191" t="s">
         <v>2</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B192" t="s">
         <v>4</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B195" t="s">
         <v>3</v>
@@ -4087,7 +4087,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B197" t="s">
         <v>3</v>
@@ -4098,7 +4098,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B198" t="s">
         <v>3</v>
@@ -4109,7 +4109,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B199" t="s">
         <v>3</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B200" t="s">
         <v>3</v>
@@ -4131,7 +4131,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B201" t="s">
         <v>3</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B203" t="s">
         <v>3</v>
@@ -4175,7 +4175,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B205" t="s">
         <v>5</v>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B206" t="s">
         <v>5</v>
@@ -4197,7 +4197,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B207" t="s">
         <v>5</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B208" t="s">
         <v>5</v>
@@ -4219,7 +4219,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B209" t="s">
         <v>5</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B210" t="s">
         <v>5</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B211" t="s">
         <v>5</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B212" t="s">
         <v>5</v>
@@ -4263,7 +4263,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B213" t="s">
         <v>5</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B214" t="s">
         <v>5</v>
@@ -4285,10 +4285,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B215" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B216" t="s">
         <v>6</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B217" t="s">
         <v>3</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B218" t="s">
         <v>7</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B219" t="s">
         <v>7</v>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B220" t="s">
         <v>7</v>
@@ -4351,7 +4351,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B221" t="s">
         <v>7</v>
@@ -4362,7 +4362,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B222" t="s">
         <v>7</v>
@@ -4373,10 +4373,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B223" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -4384,10 +4384,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B224" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -4395,10 +4395,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B225" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -4406,10 +4406,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B226" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B227" t="s">
         <v>10</v>
@@ -4428,7 +4428,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B228" t="s">
         <v>7</v>
@@ -4439,7 +4439,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B229" t="s">
         <v>10</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B230" t="s">
         <v>8</v>
@@ -4461,7 +4461,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B231" t="s">
         <v>6</v>
@@ -4472,7 +4472,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B232" t="s">
         <v>6</v>
@@ -4483,7 +4483,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B233" t="s">
         <v>7</v>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B234" t="s">
         <v>6</v>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B235" t="s">
         <v>9</v>
@@ -4516,10 +4516,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B236" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C236">
         <v>0</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B237" t="s">
         <v>7</v>
@@ -4538,10 +4538,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B238" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C238">
         <v>1</v>
@@ -4549,10 +4549,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B239" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C239">
         <v>1</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B240" t="s">
         <v>7</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B241" t="s">
         <v>10</v>
@@ -4582,7 +4582,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B242" t="s">
         <v>9</v>
@@ -4593,10 +4593,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B243" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C243">
         <v>0</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B244" t="s">
         <v>16</v>
@@ -4615,7 +4615,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B245" t="s">
         <v>9</v>
@@ -4626,10 +4626,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B246" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C246">
         <v>0</v>
@@ -4637,10 +4637,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B247" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C247">
         <v>0</v>
@@ -4648,7 +4648,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B248" t="s">
         <v>6</v>
@@ -4659,7 +4659,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B249" t="s">
         <v>6</v>
@@ -4670,10 +4670,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B250" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C250">
         <v>0</v>
@@ -4681,10 +4681,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B251" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -4692,10 +4692,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B252" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B253" t="s">
         <v>7</v>
@@ -4714,7 +4714,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B254" t="s">
         <v>10</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B255" t="s">
         <v>6</v>
@@ -4736,10 +4736,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B256" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -4747,10 +4747,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B257" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -4758,10 +4758,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B258" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -4769,7 +4769,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B259" t="s">
         <v>6</v>
@@ -4780,7 +4780,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B260" t="s">
         <v>7</v>
@@ -4791,10 +4791,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B261" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B262" t="s">
         <v>7</v>
@@ -4813,10 +4813,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B263" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C263">
         <v>0</v>
@@ -4824,7 +4824,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B264" t="s">
         <v>6</v>
@@ -4835,7 +4835,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B265" t="s">
         <v>9</v>
@@ -4846,10 +4846,10 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B266" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C266">
         <v>1</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B267" t="s">
         <v>6</v>
@@ -4868,10 +4868,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B268" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C268">
         <v>1</v>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B269" t="s">
         <v>6</v>
@@ -4890,7 +4890,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B270" t="s">
         <v>7</v>
@@ -4901,10 +4901,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B271" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C271">
         <v>1</v>
@@ -4912,7 +4912,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B272" t="s">
         <v>6</v>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B273" t="s">
         <v>9</v>
@@ -4934,7 +4934,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B274" t="s">
         <v>6</v>
@@ -4945,7 +4945,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B275" t="s">
         <v>7</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B276" t="s">
         <v>9</v>
@@ -4967,7 +4967,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B277" t="s">
         <v>9</v>
@@ -4978,7 +4978,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B278" t="s">
         <v>6</v>
@@ -4989,7 +4989,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B279" t="s">
         <v>16</v>
@@ -5000,7 +5000,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B280" t="s">
         <v>9</v>
@@ -5011,7 +5011,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B281" t="s">
         <v>9</v>
@@ -5022,7 +5022,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B282" t="s">
         <v>7</v>
@@ -5033,10 +5033,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B283" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C283">
         <v>1</v>
@@ -5044,7 +5044,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B284" t="s">
         <v>9</v>
@@ -5055,7 +5055,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B285" t="s">
         <v>9</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B286" t="s">
         <v>11</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B287" t="s">
         <v>8</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B288" t="s">
         <v>6</v>
@@ -5099,7 +5099,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B289" t="s">
         <v>9</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B290" t="s">
         <v>6</v>
@@ -5121,7 +5121,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B291" t="s">
         <v>6</v>
@@ -5132,7 +5132,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B292" t="s">
         <v>9</v>
@@ -5143,10 +5143,10 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B293" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C293">
         <v>1</v>
@@ -5154,10 +5154,10 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B294" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C294">
         <v>1</v>
@@ -5165,7 +5165,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B295" t="s">
         <v>12</v>
@@ -5176,7 +5176,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B296" t="s">
         <v>17</v>
@@ -5187,7 +5187,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B297" t="s">
         <v>9</v>
@@ -5198,7 +5198,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B298" t="s">
         <v>14</v>
@@ -5209,7 +5209,7 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B299" t="s">
         <v>6</v>
@@ -5220,7 +5220,7 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B300" t="s">
         <v>17</v>
@@ -5231,10 +5231,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B301" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C301">
         <v>1</v>
@@ -5242,7 +5242,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B302" t="s">
         <v>9</v>
@@ -5253,7 +5253,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B303" t="s">
         <v>8</v>
@@ -5264,7 +5264,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B304" t="s">
         <v>17</v>
@@ -5275,10 +5275,10 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B305" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C305">
         <v>1</v>
@@ -5286,10 +5286,10 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B306" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C306">
         <v>0</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B307" t="s">
         <v>17</v>
@@ -5308,10 +5308,10 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B308" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C308">
         <v>1</v>
@@ -5319,7 +5319,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B309" t="s">
         <v>11</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B310" t="s">
         <v>9</v>
@@ -5341,7 +5341,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B311" t="s">
         <v>9</v>
@@ -5352,10 +5352,10 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B312" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C312">
         <v>0</v>
@@ -5363,7 +5363,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B313" t="s">
         <v>6</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B314" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C314">
         <v>1</v>
@@ -5385,7 +5385,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B315" t="s">
         <v>17</v>
@@ -5396,7 +5396,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B316" t="s">
         <v>9</v>
@@ -5407,7 +5407,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B317" t="s">
         <v>13</v>
@@ -5418,7 +5418,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B318" t="s">
         <v>14</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B319" t="s">
         <v>17</v>
@@ -5440,7 +5440,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B320" t="s">
         <v>17</v>
@@ -5451,10 +5451,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B321" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C321">
         <v>1</v>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B322" t="s">
         <v>11</v>
@@ -5473,7 +5473,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B323" t="s">
         <v>17</v>
@@ -5484,10 +5484,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B324" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C324">
         <v>1</v>
@@ -5495,10 +5495,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B325" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C325">
         <v>1</v>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B326" t="s">
         <v>6</v>
@@ -5517,7 +5517,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B327" t="s">
         <v>11</v>
@@ -5528,7 +5528,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B328" t="s">
         <v>6</v>
@@ -5539,7 +5539,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B329" t="s">
         <v>8</v>
@@ -5550,10 +5550,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B330" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C330">
         <v>1</v>
@@ -5561,7 +5561,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B331" t="s">
         <v>6</v>
@@ -5572,7 +5572,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B332" t="s">
         <v>17</v>
@@ -5583,7 +5583,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B333" t="s">
         <v>6</v>
@@ -5594,10 +5594,10 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B334" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C334">
         <v>1</v>
@@ -5605,7 +5605,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B335" t="s">
         <v>6</v>
@@ -5616,7 +5616,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B336" t="s">
         <v>8</v>
@@ -5627,7 +5627,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B337" t="s">
         <v>15</v>
@@ -5638,7 +5638,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B338" t="s">
         <v>8</v>
@@ -5649,7 +5649,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B339" t="s">
         <v>6</v>
@@ -5660,7 +5660,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B340" t="s">
         <v>8</v>
@@ -5671,7 +5671,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B341" t="s">
         <v>6</v>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B342" t="s">
         <v>15</v>
@@ -5693,10 +5693,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B343" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C343">
         <v>1</v>
@@ -5704,7 +5704,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B344" t="s">
         <v>6</v>
@@ -5715,7 +5715,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B345" t="s">
         <v>8</v>
@@ -5726,10 +5726,10 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B346" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C346">
         <v>1</v>
@@ -5737,7 +5737,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B347" t="s">
         <v>6</v>
@@ -5748,7 +5748,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B348" t="s">
         <v>9</v>
@@ -5759,7 +5759,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B349" t="s">
         <v>6</v>
@@ -5770,7 +5770,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B350" t="s">
         <v>6</v>
@@ -5781,10 +5781,10 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B351" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C351">
         <v>1</v>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B352" t="s">
         <v>8</v>
@@ -5803,7 +5803,7 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B353" t="s">
         <v>8</v>
@@ -5814,7 +5814,7 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B354" t="s">
         <v>9</v>
@@ -5825,7 +5825,7 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B355" t="s">
         <v>16</v>
@@ -5836,10 +5836,10 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B356" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C356">
         <v>1</v>
@@ -5847,10 +5847,10 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B357" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C357">
         <v>1</v>
@@ -5858,7 +5858,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B358" t="s">
         <v>6</v>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B359" t="s">
         <v>6</v>
@@ -5880,10 +5880,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B360" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C360">
         <v>1</v>
@@ -5891,10 +5891,10 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B361" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C361">
         <v>1</v>
@@ -5902,10 +5902,10 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B362" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C362">
         <v>1</v>
@@ -5913,10 +5913,10 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B363" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C363">
         <v>0</v>
@@ -5924,7 +5924,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B364" t="s">
         <v>16</v>
@@ -5935,10 +5935,10 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B365" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C365">
         <v>1</v>
@@ -5946,10 +5946,10 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B366" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C366">
         <v>1</v>
@@ -5957,10 +5957,10 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B367" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C367">
         <v>1</v>
@@ -5968,10 +5968,10 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B368" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C368">
         <v>1</v>
@@ -5979,7 +5979,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B369" t="s">
         <v>17</v>
@@ -5990,7 +5990,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B370" t="s">
         <v>9</v>
@@ -6001,7 +6001,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B371" t="s">
         <v>6</v>
@@ -6012,10 +6012,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B372" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C372">
         <v>1</v>
@@ -6023,7 +6023,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B373" t="s">
         <v>18</v>
@@ -6034,10 +6034,10 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B374" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C374">
         <v>1</v>
@@ -6045,10 +6045,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B375" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C375">
         <v>1</v>
@@ -6056,7 +6056,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B376" t="s">
         <v>17</v>
@@ -6067,10 +6067,10 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B377" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C377">
         <v>1</v>
@@ -6078,10 +6078,10 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B378" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C378">
         <v>1</v>
@@ -6089,7 +6089,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B379" t="s">
         <v>16</v>
@@ -6100,10 +6100,10 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B380" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C380">
         <v>1</v>
@@ -6111,7 +6111,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B381" t="s">
         <v>6</v>
@@ -6122,7 +6122,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B382" t="s">
         <v>19</v>
@@ -6133,10 +6133,10 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B383" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C383">
         <v>0</v>
@@ -6144,7 +6144,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B384" t="s">
         <v>18</v>
@@ -6155,7 +6155,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B385" t="s">
         <v>20</v>
@@ -6166,10 +6166,10 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B386" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C386">
         <v>0</v>
@@ -6177,7 +6177,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B387" t="s">
         <v>11</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B388" t="s">
         <v>18</v>
@@ -6199,7 +6199,7 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B389" t="s">
         <v>17</v>
@@ -6210,10 +6210,10 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B390" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C390">
         <v>0</v>
@@ -6221,7 +6221,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B391" t="s">
         <v>18</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B392" t="s">
         <v>18</v>
@@ -6243,7 +6243,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B393" t="s">
         <v>18</v>
@@ -6254,10 +6254,10 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B394" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C394">
         <v>0</v>
@@ -6265,10 +6265,10 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B395" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C395">
         <v>1</v>
@@ -6276,10 +6276,10 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B396" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C396">
         <v>1</v>
@@ -6287,7 +6287,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B397" t="s">
         <v>14</v>
@@ -6298,7 +6298,7 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B398" t="s">
         <v>18</v>
@@ -6309,10 +6309,10 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B399" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C399">
         <v>1</v>
@@ -6320,7 +6320,7 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B400" t="s">
         <v>20</v>
@@ -6331,7 +6331,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B401" t="s">
         <v>18</v>
@@ -6342,10 +6342,10 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B402" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C402">
         <v>1</v>
@@ -6353,7 +6353,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B403" t="s">
         <v>18</v>
@@ -6364,10 +6364,10 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B404" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -6375,10 +6375,10 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B405" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C405">
         <v>1</v>
@@ -6386,10 +6386,10 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B406" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C406">
         <v>1</v>
@@ -6397,7 +6397,7 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B407" t="s">
         <v>6</v>
@@ -6408,10 +6408,10 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B408" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C408">
         <v>1</v>
@@ -6419,10 +6419,10 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B409" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C409">
         <v>1</v>
@@ -6430,10 +6430,10 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B410" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C410">
         <v>1</v>
@@ -6441,10 +6441,10 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B411" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C411">
         <v>1</v>
@@ -6452,10 +6452,10 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B412" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C412">
         <v>1</v>
@@ -6463,10 +6463,10 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B413" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C413">
         <v>1</v>
@@ -6474,10 +6474,10 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B414" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C414">
         <v>1</v>
@@ -6485,10 +6485,10 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B415" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C415">
         <v>1</v>
@@ -6496,10 +6496,10 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B416" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C416">
         <v>1</v>
@@ -6507,10 +6507,10 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B417" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C417">
         <v>1</v>
@@ -6518,10 +6518,10 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B418" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C418">
         <v>1</v>
@@ -6529,10 +6529,10 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B419" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C419">
         <v>1</v>
@@ -6540,10 +6540,10 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B420" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C420">
         <v>1</v>
@@ -6551,10 +6551,10 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B421" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C421">
         <v>1</v>
@@ -6562,10 +6562,10 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B422" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C422">
         <v>1</v>
@@ -6573,10 +6573,10 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B423" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C423">
         <v>1</v>
@@ -6584,10 +6584,10 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B424" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C424">
         <v>1</v>
@@ -6595,10 +6595,10 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B425" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C425">
         <v>1</v>
@@ -6606,10 +6606,10 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B426" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C426">
         <v>1</v>
@@ -6617,10 +6617,10 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B427" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C427">
         <v>1</v>
@@ -6628,10 +6628,10 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B428" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C428">
         <v>1</v>
@@ -6639,10 +6639,10 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B429" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C429">
         <v>1</v>
@@ -6650,10 +6650,10 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B430" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C430">
         <v>1</v>
@@ -6661,10 +6661,10 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B431" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C431">
         <v>1</v>
@@ -6672,10 +6672,10 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B432" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C432">
         <v>1</v>
@@ -6683,10 +6683,10 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B433" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C433">
         <v>1</v>
@@ -6694,10 +6694,10 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B434" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C434">
         <v>1</v>
@@ -6705,10 +6705,10 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B435" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C435">
         <v>1</v>
@@ -6716,7 +6716,7 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B436" t="s">
         <v>6</v>
@@ -6727,10 +6727,10 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B437" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C437">
         <v>1</v>
@@ -6738,10 +6738,10 @@
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B438" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C438">
         <v>1</v>
@@ -6749,7 +6749,7 @@
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B439" t="s">
         <v>18</v>
@@ -6760,10 +6760,10 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B440" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C440">
         <v>1</v>
@@ -6771,10 +6771,10 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B441" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C441">
         <v>1</v>
@@ -6782,10 +6782,10 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B442" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C442">
         <v>1</v>
@@ -6793,10 +6793,10 @@
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B443" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C443">
         <v>1</v>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B444" t="s">
         <v>19</v>
@@ -6815,7 +6815,7 @@
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B445" t="s">
         <v>14</v>
@@ -6826,10 +6826,10 @@
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B446" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C446">
         <v>1</v>
@@ -6837,10 +6837,10 @@
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B447" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C447">
         <v>1</v>
@@ -6848,10 +6848,10 @@
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B448" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C448">
         <v>1</v>
@@ -6859,10 +6859,10 @@
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B449" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C449">
         <v>0</v>
@@ -6870,7 +6870,7 @@
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B450" t="s">
         <v>9</v>
@@ -6881,7 +6881,7 @@
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B451" t="s">
         <v>14</v>
@@ -6892,7 +6892,7 @@
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B452" t="s">
         <v>19</v>
@@ -6903,7 +6903,7 @@
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B453" t="s">
         <v>16</v>
@@ -6914,7 +6914,7 @@
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B454" t="s">
         <v>20</v>
@@ -6925,7 +6925,7 @@
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B455" t="s">
         <v>9</v>
@@ -6936,10 +6936,10 @@
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B456" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C456">
         <v>0</v>
@@ -6947,10 +6947,10 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B457" t="s">
-        <v>21</v>
+        <v>363</v>
       </c>
       <c r="C457">
         <v>0</v>
@@ -6958,7 +6958,7 @@
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B458" t="s">
         <v>6</v>
@@ -6969,10 +6969,10 @@
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B459" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C459">
         <v>0</v>
@@ -6980,7 +6980,7 @@
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B460" t="s">
         <v>14</v>
@@ -6991,10 +6991,10 @@
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B461" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C461">
         <v>0</v>
@@ -7002,7 +7002,7 @@
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B462" t="s">
         <v>17</v>
@@ -7013,10 +7013,10 @@
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B463" t="s">
-        <v>21</v>
+        <v>363</v>
       </c>
       <c r="C463">
         <v>0</v>
@@ -7024,10 +7024,10 @@
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B464" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C464">
         <v>1</v>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B465" t="s">
         <v>12</v>
@@ -7046,7 +7046,7 @@
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B466" t="s">
         <v>12</v>
@@ -7057,7 +7057,7 @@
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B467" t="s">
         <v>12</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B468" t="s">
         <v>12</v>
@@ -7079,10 +7079,10 @@
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B469" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C469">
         <v>0</v>
@@ -7090,10 +7090,10 @@
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B470" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C470">
         <v>0</v>
@@ -7101,7 +7101,7 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B471" t="s">
         <v>12</v>
@@ -7112,10 +7112,10 @@
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B472" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C472">
         <v>0</v>
@@ -7123,7 +7123,7 @@
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B473" t="s">
         <v>12</v>
@@ -7134,7 +7134,7 @@
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B474" t="s">
         <v>12</v>
@@ -7145,7 +7145,7 @@
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B475" t="s">
         <v>12</v>
@@ -7156,10 +7156,10 @@
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B476" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C476">
         <v>0</v>
@@ -7167,7 +7167,7 @@
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B477" t="s">
         <v>12</v>
@@ -7178,7 +7178,7 @@
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B478" t="s">
         <v>9</v>
@@ -7189,7 +7189,7 @@
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B479" t="s">
         <v>6</v>
@@ -7200,7 +7200,7 @@
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B480" t="s">
         <v>6</v>
@@ -7211,7 +7211,7 @@
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B481" t="s">
         <v>6</v>
@@ -7222,7 +7222,7 @@
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B482" t="s">
         <v>9</v>
@@ -7233,7 +7233,7 @@
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B483" t="s">
         <v>9</v>
@@ -7244,7 +7244,7 @@
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B484" t="s">
         <v>18</v>
@@ -7255,7 +7255,7 @@
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B485" t="s">
         <v>4</v>

</xml_diff>